<commit_message>
update data mining goals
</commit_message>
<xml_diff>
--- a/kaggle.com/Santander_Customer_Transaction_Prediction/Business_Understanding/Business_Understanding.xlsx
+++ b/kaggle.com/Santander_Customer_Transaction_Prediction/Business_Understanding/Business_Understanding.xlsx
@@ -8,25 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbwes\Documents\Programmierworkspaces\Python\DataScienceProjects-1\kaggle.com\Santander_Customer_Transaction_Prediction\Business_Understanding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E987BA-B8D2-4ADF-BE31-042815143C2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9603B3-BD09-4A23-80F0-D2A4E8B1BECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Business_Understanding" sheetId="1" r:id="rId1"/>
     <sheet name="Data Mining Goals" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Business Understanding</t>
   </si>
@@ -90,12 +96,69 @@
   <si>
     <t>*Submission format:</t>
   </si>
+  <si>
+    <t>*What is the ROC curve?</t>
+  </si>
+  <si>
+    <t>*Confusion Matrix</t>
+  </si>
+  <si>
+    <t>Predicted</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>*An ROC curve (receiver operating characteristic curve) is a graph showing the performance of a classification model at all classification thresholds</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/machine-learning/crash-course/classification/roc-and-auc</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>*Consists of True Positive Rate (TPR) and False Positive Rate (FPR)</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/understanding-auc-roc-curve-68b2303cc9c5</t>
+  </si>
+  <si>
+    <t>*ROC is a probability curve and AUC represents degree or measure of separability. It tells how much a model is capable of distinguishing between classes. Higher the AUC, better the model is at predicting 0s as 0s and 1s as 1s</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TPR/Recall/Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*By measuring the TPR and FPR for different thresholds, we establish the ROC </t>
+  </si>
+  <si>
+    <t>Area under the curve (AUC)</t>
+  </si>
+  <si>
+    <t>*We consider our journey to be a data mining success if the AUC is at least at 0,8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +189,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -147,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -244,11 +314,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -285,11 +371,124 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -308,13 +507,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>580836</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>114148</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -346,6 +545,705 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447264</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>9200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44F21028-AC7E-4F0E-972F-6C994356A2AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="8191500"/>
+          <a:ext cx="3285714" cy="2600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Gerader Verbinder 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{013CDAF4-A58A-4ED7-9F94-42A88639388B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2476500" y="9334500"/>
+          <a:ext cx="304800" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Gerader Verbinder 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78E5F3F7-9F40-49ED-9067-99F20A4F47ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2628900" y="9925050"/>
+          <a:ext cx="161925" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Gerader Verbinder 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9F45B41-50D2-4D29-840E-11DE18B9811E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2962275" y="9020175"/>
+          <a:ext cx="161925" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Gerader Verbinder 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{585252D5-3259-4B5E-93CF-4529ED6F0D81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3238500" y="8877300"/>
+          <a:ext cx="152400" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Gerader Verbinder 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CE626ED-8DAE-4D48-8C49-545A51156967}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2933700" y="10020301"/>
+          <a:ext cx="114300" cy="409574"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Gerader Verbinder 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C9C5F0-BA4C-4BE9-A1D9-B321F80062CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3486150" y="8705851"/>
+          <a:ext cx="152400" cy="676274"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Gerader Verbinder 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF88543C-645B-4A4C-9A69-80CE6CB38CA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3257550" y="10001251"/>
+          <a:ext cx="85725" cy="390524"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Gerader Verbinder 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67203A0E-85A2-4059-AE8B-B87AD15605A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3571875" y="10001251"/>
+          <a:ext cx="85725" cy="390524"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Gerader Verbinder 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FD5998B-104F-468B-82BD-E2DA67D1FF13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3876675" y="9267825"/>
+          <a:ext cx="247650" cy="1133475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Gerader Verbinder 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEFA61E-29FE-4B21-94A3-0C7557CFDA3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3762375" y="8972551"/>
+          <a:ext cx="85725" cy="390524"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Gerader Verbinder 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F17EA0EE-478E-45F7-BF13-BECDEB883935}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4200525" y="9239250"/>
+          <a:ext cx="247650" cy="1133475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Gerader Verbinder 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77FEA202-EA4C-4F95-A843-C8256E6C504B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4495800" y="9229725"/>
+          <a:ext cx="247650" cy="1133475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Gerader Verbinder 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D5C1AC1-3250-4D9D-A4BB-CAD806E49867}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4752975" y="9001125"/>
+          <a:ext cx="1143000" cy="381001"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -848,13 +1746,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050AC8F5-7F2A-4AF3-AFBF-AA8438D5051F}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
@@ -895,20 +1793,209 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>15</v>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="F35" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="K35" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" s="16"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="F36" s="17">
+        <v>1</v>
+      </c>
+      <c r="G36" s="17">
+        <v>0</v>
+      </c>
+      <c r="K36" s="17">
+        <v>1</v>
+      </c>
+      <c r="L36" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D37" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="17">
+        <v>1</v>
+      </c>
+      <c r="F37" s="17">
+        <v>10109</v>
+      </c>
+      <c r="G37" s="17">
+        <v>1013</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="17">
+        <v>1</v>
+      </c>
+      <c r="K37" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D38" s="18"/>
+      <c r="E38" s="17">
+        <v>0</v>
+      </c>
+      <c r="F38" s="17">
+        <v>1486</v>
+      </c>
+      <c r="G38" s="17">
+        <v>2045</v>
+      </c>
+      <c r="I38" s="18"/>
+      <c r="J38" s="17">
+        <v>0</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="L38" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="19">
+        <f>F37/SUM(F37:G37)</f>
+        <v>0.90891925912605642</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="19">
+        <f>F38/SUM(F38:G38)</f>
+        <v>0.42084395355423393</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="K35:L35"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F36:G36">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37:E38">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36:L36">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L36">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37:J38">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>